<commit_message>
saving all the file
</commit_message>
<xml_diff>
--- a/Practice_problem/Book1.xlsx
+++ b/Practice_problem/Book1.xlsx
@@ -1,35 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Python\Practice_problem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="New sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Master_sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+  <si>
+    <t>psnumber</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>emai</t>
+  </si>
+  <si>
+    <t>ankit</t>
+  </si>
+  <si>
+    <t>ankit@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,84 +75,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,62 +384,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Aadrika</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Adwaita</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Satyajit</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bivas</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>99003720</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>99003721</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>99003722</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>99003723</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>99003720</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>99003720</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>99003720</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3:C8" r:id="rId2" display="ankit@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
saving all the work
</commit_message>
<xml_diff>
--- a/Practice_problem/Book1.xlsx
+++ b/Practice_problem/Book1.xlsx
@@ -1,58 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Python\Practice_problem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivam\PycharmProjects\Python_Practice\Practice_problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Master_sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Master6" sheetId="2" r:id="rId2"/>
+    <sheet name="Master5" sheetId="3" r:id="rId3"/>
+    <sheet name="Master4" sheetId="4" r:id="rId4"/>
+    <sheet name="Master3" sheetId="5" r:id="rId5"/>
+    <sheet name="Master2" sheetId="6" r:id="rId6"/>
+    <sheet name="Master1" sheetId="7" r:id="rId7"/>
+    <sheet name="Master" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>psnumber</t>
+    <t xml:space="preserve">id </t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>emai</t>
+    <t>email</t>
   </si>
   <si>
-    <t>ankit</t>
+    <t>sravan</t>
   </si>
   <si>
-    <t>ankit@gmail.com</t>
+    <t>abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,16 +73,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,16 +380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -409,88 +401,17 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>99003720</v>
+        <v>99003758</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>99003721</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>99003722</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>99003723</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>99003720</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>99003720</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>99003720</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3:C8" r:id="rId2" display="ankit@gmail.com"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -503,6 +424,77 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>